<commit_message>
added for project sheet
</commit_message>
<xml_diff>
--- a/PPT/ProjectSheet.xlsx
+++ b/PPT/ProjectSheet.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Mock interview Schedules" sheetId="2" r:id="rId2"/>
     <sheet name="Project-1" sheetId="3" r:id="rId3"/>
     <sheet name="Project-2" sheetId="4" r:id="rId4"/>
+    <sheet name="Resume_CV Preparation" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Pramod</t>
   </si>
@@ -212,6 +213,12 @@
   </si>
   <si>
     <t>Fetch/Get button missing</t>
+  </si>
+  <si>
+    <t>Shared and given 1st review</t>
+  </si>
+  <si>
+    <t>Review comments Implemented or not</t>
   </si>
 </sst>
 </file>
@@ -578,7 +585,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -767,7 +774,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1087,4 +1094,95 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
second review assessment details
</commit_message>
<xml_diff>
--- a/PPT/ProjectSheet.xlsx
+++ b/PPT/ProjectSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tentaive Dates" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>Pramod</t>
   </si>
@@ -65,12 +65,6 @@
     <t>Final Review</t>
   </si>
   <si>
-    <t>Second Review</t>
-  </si>
-  <si>
-    <t>First Review</t>
-  </si>
-  <si>
     <t>Date Final Review/Submission</t>
   </si>
   <si>
@@ -219,13 +213,46 @@
   </si>
   <si>
     <t>Review comments Implemented or not</t>
+  </si>
+  <si>
+    <t>Input data from the Layout need to convert appropriate datatype</t>
+  </si>
+  <si>
+    <t>Once save button click, data should be saved in map</t>
+  </si>
+  <si>
+    <t>Once map grows, from the exit layout data need to fetch</t>
+  </si>
+  <si>
+    <t>After conversion to appropriate data type start working the logic part</t>
+  </si>
+  <si>
+    <t>What are the fields that should be mandatorly required</t>
+  </si>
+  <si>
+    <t>Second Review Assessment -Phase 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validataion- Phase 2 </t>
+  </si>
+  <si>
+    <t>parking person without submit the (vehicle number, type,time) data should not get save</t>
+  </si>
+  <si>
+    <t>If data is empty, u should give a message, "Please enter valid details"</t>
+  </si>
+  <si>
+    <t>Second Review (35%)</t>
+  </si>
+  <si>
+    <t>First Review(25%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +275,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -263,12 +298,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -279,14 +329,18 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -592,174 +646,241 @@
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="31.42578125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="7">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="7">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="B17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B18" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" t="s">
-        <v>22</v>
-      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -785,18 +906,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>23</v>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>44955</v>
       </c>
     </row>
@@ -804,7 +925,7 @@
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>44955</v>
       </c>
     </row>
@@ -812,7 +933,7 @@
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>44954</v>
       </c>
     </row>
@@ -820,7 +941,7 @@
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>44952</v>
       </c>
     </row>
@@ -828,7 +949,7 @@
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>44952</v>
       </c>
     </row>
@@ -836,7 +957,7 @@
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>44956</v>
       </c>
     </row>
@@ -844,7 +965,7 @@
       <c r="A8" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>44954</v>
       </c>
     </row>
@@ -853,7 +974,7 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -889,15 +1010,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="37" customWidth="1"/>
     <col min="4" max="4" width="24" customWidth="1"/>
@@ -905,74 +1026,74 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>28</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -982,105 +1103,157 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" s="1">
         <v>0.5</v>
       </c>
     </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1146,15 +1319,15 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>

<commit_message>
todays class discussion topic
</commit_message>
<xml_diff>
--- a/PPT/ProjectSheet.xlsx
+++ b/PPT/ProjectSheet.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>Pramod</t>
   </si>
@@ -71,18 +71,12 @@
     <t>Date First Review</t>
   </si>
   <si>
-    <t>29/01/2023</t>
-  </si>
-  <si>
     <t>15/01/2023</t>
   </si>
   <si>
     <t>Date Second Review</t>
   </si>
   <si>
-    <t>22/01/2023</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -249,6 +243,9 @@
   </si>
   <si>
     <t>Completed</t>
+  </si>
+  <si>
+    <t>25/02/2023</t>
   </si>
 </sst>
 </file>
@@ -332,7 +329,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -344,6 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -642,7 +640,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -663,16 +661,16 @@
         <v>9</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -683,7 +681,7 @@
         <v>0.25</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -697,7 +695,7 @@
         <v>0.25</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
@@ -711,7 +709,7 @@
         <v>0.25</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -722,7 +720,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="7">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -737,7 +735,7 @@
         <v>0.25</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
@@ -751,7 +749,7 @@
         <v>0.25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
@@ -765,7 +763,7 @@
         <v>0.25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
@@ -773,16 +771,18 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B9" s="7">
         <v>0</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -792,7 +792,9 @@
       <c r="B10" s="7">
         <v>0</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -804,7 +806,9 @@
       <c r="B11" s="7">
         <v>0</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -817,7 +821,7 @@
         <v>0.25</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -831,7 +835,7 @@
         <v>0.25</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -857,8 +861,8 @@
       <c r="A16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>17</v>
+      <c r="B16" s="11">
+        <v>44988</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
@@ -870,7 +874,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -879,10 +883,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
@@ -902,7 +906,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -917,7 +921,7 @@
         <v>8</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -941,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>44954</v>
+        <v>44962</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -957,7 +961,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="4">
-        <v>44952</v>
+        <v>44962</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -973,7 +977,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="4">
-        <v>44954</v>
+        <v>44975</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -981,22 +985,31 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
+      </c>
+      <c r="B12" s="4">
+        <v>44972</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1033,74 +1046,74 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1110,96 +1123,96 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="C18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1209,7 +1222,7 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35" s="1">
         <v>0.25</v>
@@ -1217,27 +1230,27 @@
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B41" s="1">
         <v>0.1</v>
@@ -1245,17 +1258,17 @@
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1281,7 +1294,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1321,24 +1334,27 @@
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:4">

</xml_diff>